<commit_message>
update task and document about test question (test question need to be classified )
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Task No.</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>Phân lọai các câu hỏi trong chương trình</t>
+  </si>
+  <si>
+    <t>17/11</t>
+  </si>
+  <si>
+    <t>on processing</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
   <dimension ref="A3:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -750,17 +759,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="33">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5">

</xml_diff>

<commit_message>
CLEAN PROJECT FOLDER !
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Task No.</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Module rút bộ ba quan hệ theo từ</t>
   </si>
   <si>
-    <t>DELAY</t>
-  </si>
-  <si>
     <t>19/11</t>
   </si>
   <si>
@@ -103,6 +100,27 @@
   </si>
   <si>
     <t>on processing</t>
+  </si>
+  <si>
+    <t>nearly done</t>
+  </si>
+  <si>
+    <t>Hưng</t>
+  </si>
+  <si>
+    <t>Hoang &amp; Hung</t>
+  </si>
+  <si>
+    <t>Module liệt kê bộ ba</t>
+  </si>
+  <si>
+    <t>Module nhận biết thực thể</t>
+  </si>
+  <si>
+    <t>Module sinh câu truy vấn</t>
+  </si>
+  <si>
+    <t>12/12</t>
   </si>
 </sst>
 </file>
@@ -130,7 +148,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,12 +182,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,8 +263,7 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -669,8 +680,8 @@
         <v>1</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="11" t="s">
-        <v>14</v>
+      <c r="G7" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -691,8 +702,8 @@
         <v>0.05</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="16" t="s">
-        <v>22</v>
+      <c r="G8" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -713,8 +724,8 @@
         <v>0.75</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="11" t="s">
-        <v>14</v>
+      <c r="G9" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -729,13 +740,15 @@
         <v>10</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="8">
         <v>0.5</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5">
@@ -743,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -755,8 +768,8 @@
         <v>0.8</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="17" t="s">
-        <v>25</v>
+      <c r="G11" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="33">
@@ -765,16 +778,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="3" t="s">
@@ -786,36 +799,66 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.9</v>
+      </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="8"/>
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5">

</xml_diff>

<commit_message>
- delete un-use Source code/XMLConfig - update tasks : task doned (100%) - delete file update DBLP_SQL.txt ( already have in main source)
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Task No.</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Process</t>
   </si>
   <si>
-    <t>Tạm ổn</t>
-  </si>
-  <si>
     <t>Triển khai module hỏi đáp</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>26/11</t>
   </si>
   <si>
-    <t>hủy</t>
-  </si>
-  <si>
     <t>05/11</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>on processing</t>
   </si>
   <si>
-    <t>nearly done</t>
-  </si>
-  <si>
     <t>Hưng</t>
   </si>
   <si>
@@ -121,6 +112,24 @@
   </si>
   <si>
     <t>12/12</t>
+  </si>
+  <si>
+    <t>Đọc bài báo - "Triplet extraction from sentence" -  "Question Answering Based on Semantic Graphs"</t>
+  </si>
+  <si>
+    <t>3/1</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>Các vấn đề trong tương tác người dùng ở hệ thống hỏi đáp</t>
+  </si>
+  <si>
+    <t>10/1</t>
+  </si>
+  <si>
+    <t>Tích hợp module hỏi đáp vào hệ thống</t>
   </si>
 </sst>
 </file>
@@ -142,13 +151,15 @@
       <family val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="13"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,18 +192,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -226,11 +243,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -252,9 +295,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -263,7 +303,37 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:G54"/>
+  <dimension ref="A3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -569,14 +639,14 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="14" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="9.140625" style="10"/>
     <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,7 +656,7 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -597,7 +667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="66">
+    <row r="4" spans="1:8" ht="66">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -607,18 +677,21 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="66">
+      <c r="G4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="22">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="66">
       <c r="A5" s="5">
         <f xml:space="preserve"> A4 +1</f>
         <v>2</v>
@@ -629,18 +702,19 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="66">
+      <c r="G5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" ht="66">
       <c r="A6" s="5">
         <f xml:space="preserve"> A5 +1</f>
         <v>3</v>
@@ -651,18 +725,19 @@
       <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="33">
+      <c r="G6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" ht="33">
       <c r="A7" s="5">
         <f xml:space="preserve"> A6 +1</f>
         <v>4</v>
@@ -673,393 +748,446 @@
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="5">
         <f t="shared" ref="A8:A41" si="0" xml:space="preserve"> A7 +1</f>
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>20</v>
+      <c r="D9" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="E9" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>20</v>
+      <c r="D11" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="E11" s="8">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="33">
+      <c r="G11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="33">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5">
-        <f t="shared" si="0"/>
+      <c r="D13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" ht="66">
+      <c r="A17" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="5">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="3" t="s">
+      <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="22">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="33">
+      <c r="A18" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="33">
+      <c r="A19" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="D19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="5">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="G19" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
       <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="23"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="23"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
       <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
       <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
       <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
       <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="13"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="13"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
       <c r="G32" s="3"/>
@@ -1071,7 +1199,7 @@
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="13"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
       <c r="G33" s="3"/>
@@ -1083,7 +1211,7 @@
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="13"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
       <c r="G34" s="3"/>
@@ -1095,7 +1223,7 @@
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="13"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="8"/>
       <c r="F35" s="9"/>
       <c r="G35" s="3"/>
@@ -1107,7 +1235,7 @@
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="13"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="8"/>
       <c r="F36" s="9"/>
       <c r="G36" s="3"/>
@@ -1119,7 +1247,7 @@
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="13"/>
+      <c r="D37" s="12"/>
       <c r="E37" s="8"/>
       <c r="F37" s="9"/>
       <c r="G37" s="3"/>
@@ -1131,7 +1259,7 @@
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="13"/>
+      <c r="D38" s="12"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
       <c r="G38" s="3"/>
@@ -1143,7 +1271,7 @@
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="13"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="8"/>
       <c r="F39" s="9"/>
       <c r="G39" s="3"/>
@@ -1155,7 +1283,7 @@
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="13"/>
+      <c r="D40" s="12"/>
       <c r="E40" s="8"/>
       <c r="F40" s="9"/>
       <c r="G40" s="3"/>
@@ -1167,7 +1295,7 @@
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="13"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="8"/>
       <c r="F41" s="9"/>
       <c r="G41" s="3"/>
@@ -1176,7 +1304,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="14"/>
+      <c r="D42" s="13"/>
       <c r="E42" s="3"/>
       <c r="F42" s="9"/>
       <c r="G42" s="3"/>
@@ -1185,7 +1313,7 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="14"/>
+      <c r="D43" s="13"/>
       <c r="E43" s="3"/>
       <c r="F43" s="9"/>
       <c r="G43" s="3"/>
@@ -1194,7 +1322,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="14"/>
+      <c r="D44" s="13"/>
       <c r="E44" s="3"/>
       <c r="F44" s="9"/>
       <c r="G44" s="3"/>
@@ -1203,7 +1331,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="14"/>
+      <c r="D45" s="13"/>
       <c r="E45" s="3"/>
       <c r="F45" s="9"/>
       <c r="G45" s="3"/>
@@ -1212,7 +1340,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="14"/>
+      <c r="D46" s="13"/>
       <c r="E46" s="3"/>
       <c r="F46" s="9"/>
       <c r="G46" s="3"/>
@@ -1221,7 +1349,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="14"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="3"/>
       <c r="F47" s="9"/>
       <c r="G47" s="3"/>
@@ -1230,7 +1358,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="14"/>
+      <c r="D48" s="13"/>
       <c r="E48" s="3"/>
       <c r="F48" s="9"/>
       <c r="G48" s="3"/>
@@ -1239,7 +1367,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="14"/>
+      <c r="D49" s="13"/>
       <c r="E49" s="3"/>
       <c r="F49" s="9"/>
       <c r="G49" s="3"/>
@@ -1248,7 +1376,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="14"/>
+      <c r="D50" s="13"/>
       <c r="E50" s="3"/>
       <c r="F50" s="9"/>
       <c r="G50" s="3"/>
@@ -1257,7 +1385,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="14"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="3"/>
       <c r="F51" s="9"/>
       <c r="G51" s="3"/>
@@ -1266,7 +1394,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="14"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="3"/>
       <c r="F52" s="9"/>
       <c r="G52" s="3"/>
@@ -1275,7 +1403,7 @@
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="14"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="3"/>
       <c r="F53" s="9"/>
       <c r="G53" s="3"/>
@@ -1284,12 +1412,16 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="14"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="3"/>
       <c r="F54" s="9"/>
       <c r="G54" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H4:H15"/>
+    <mergeCell ref="H17:H28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update tasks for Tet Holiday
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>Task No.</t>
   </si>
@@ -366,6 +366,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -374,33 +401,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -710,7 +710,7 @@
     <col min="4" max="4" width="8.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="14.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="25" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -731,7 +731,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -752,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="28">
         <v>2010</v>
       </c>
     </row>
@@ -777,10 +777,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="20"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:8" ht="66">
       <c r="A6" s="4">
@@ -800,10 +800,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="20"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:8" ht="33">
       <c r="A7" s="4">
@@ -823,10 +823,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="20"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4">
@@ -846,10 +846,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="20"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4">
@@ -869,10 +869,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="20"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4">
@@ -892,10 +892,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4">
@@ -915,10 +915,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="4">
@@ -938,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="20"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4">
@@ -961,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="20"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4">
@@ -984,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="20"/>
+      <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4">
@@ -1007,10 +1007,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4">
@@ -1022,7 +1022,7 @@
       <c r="D16" s="16"/>
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="25"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:8" ht="66">
       <c r="A17" s="4">
@@ -1042,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="28">
         <v>2011</v>
       </c>
     </row>
@@ -1067,10 +1067,10 @@
         <v>0.1</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="20"/>
+      <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:8" ht="33">
       <c r="A19" s="4">
@@ -1090,10 +1090,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="20"/>
+      <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4">
@@ -1105,8 +1105,8 @@
       <c r="D20" s="11"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="29"/>
     </row>
     <row r="21" spans="1:8" ht="33">
       <c r="A21" s="4">
@@ -1123,13 +1123,13 @@
       <c r="E21" s="7">
         <v>0</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="29"/>
     </row>
     <row r="22" spans="1:8" ht="33">
       <c r="A22" s="4">
@@ -1139,20 +1139,22 @@
       <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="20"/>
+      <c r="G22" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4">
@@ -1171,13 +1173,13 @@
       <c r="E23" s="7">
         <v>0.05</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="20"/>
+      <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8" ht="49.5">
       <c r="A24" s="4">
@@ -1196,13 +1198,13 @@
       <c r="E24" s="7">
         <v>0.05</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="20"/>
+      <c r="H24" s="29"/>
     </row>
     <row r="25" spans="1:8" ht="33">
       <c r="A25" s="4">
@@ -1219,13 +1221,13 @@
       <c r="E25" s="7">
         <v>0.05</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="4">
@@ -1242,13 +1244,13 @@
       <c r="E26" s="7">
         <v>0</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="1:8" ht="49.5">
       <c r="A27" s="4">
@@ -1258,20 +1260,22 @@
       <c r="B27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D27" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="7">
         <v>0</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="20"/>
+      <c r="G27" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8" ht="33">
       <c r="A28" s="4">
@@ -1281,20 +1285,22 @@
       <c r="B28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D28" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E28" s="7">
         <v>0</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G28" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="H28" s="21"/>
+      <c r="G28" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
       <c r="A29" s="4">
@@ -1306,7 +1312,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="27"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="4">
@@ -1318,7 +1324,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="27"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="4">
@@ -1330,7 +1336,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4">
@@ -1342,7 +1348,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="27"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="4">
@@ -1354,7 +1360,7 @@
       <c r="D33" s="11"/>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="27"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4">
@@ -1366,7 +1372,7 @@
       <c r="D34" s="11"/>
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="27"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="4">
@@ -1378,7 +1384,7 @@
       <c r="D35" s="11"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="27"/>
+      <c r="G35" s="24"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="4">
@@ -1390,7 +1396,7 @@
       <c r="D36" s="11"/>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="27"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="4">
@@ -1402,7 +1408,7 @@
       <c r="D37" s="11"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="27"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="4">
@@ -1414,7 +1420,7 @@
       <c r="D38" s="11"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="27"/>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4">
@@ -1426,7 +1432,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="27"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="4">
@@ -1438,7 +1444,7 @@
       <c r="D40" s="11"/>
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="27"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4">
@@ -1450,7 +1456,7 @@
       <c r="D41" s="11"/>
       <c r="E41" s="7"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="27"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="3"/>
@@ -1459,7 +1465,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="3"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="27"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="3"/>
@@ -1468,7 +1474,7 @@
       <c r="D43" s="12"/>
       <c r="E43" s="3"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="3"/>
@@ -1477,7 +1483,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="3"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="27"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="3"/>
@@ -1486,7 +1492,7 @@
       <c r="D45" s="12"/>
       <c r="E45" s="3"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="27"/>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="3"/>
@@ -1495,7 +1501,7 @@
       <c r="D46" s="12"/>
       <c r="E46" s="3"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="27"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="3"/>
@@ -1504,7 +1510,7 @@
       <c r="D47" s="12"/>
       <c r="E47" s="3"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="27"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3"/>
@@ -1513,7 +1519,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="3"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="27"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="3"/>
@@ -1522,7 +1528,7 @@
       <c r="D49" s="12"/>
       <c r="E49" s="3"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="27"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="3"/>
@@ -1531,7 +1537,7 @@
       <c r="D50" s="12"/>
       <c r="E50" s="3"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="27"/>
+      <c r="G50" s="24"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="3"/>
@@ -1540,7 +1546,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="3"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="27"/>
+      <c r="G51" s="24"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="3"/>
@@ -1549,7 +1555,7 @@
       <c r="D52" s="12"/>
       <c r="E52" s="3"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="27"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="3"/>
@@ -1558,7 +1564,7 @@
       <c r="D53" s="12"/>
       <c r="E53" s="3"/>
       <c r="F53" s="8"/>
-      <c r="G53" s="27"/>
+      <c r="G53" s="24"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="3"/>
@@ -1567,7 +1573,7 @@
       <c r="D54" s="12"/>
       <c r="E54" s="3"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="27"/>
+      <c r="G54" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
task assigned done to Hoang and Hung update write paper
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>Task No.</t>
   </si>
@@ -93,9 +93,6 @@
     <t>on processing</t>
   </si>
   <si>
-    <t>Hưng</t>
-  </si>
-  <si>
     <t>Hoang &amp; Hung</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
   </si>
   <si>
     <t>28/1</t>
-  </si>
-  <si>
-    <t>waiting</t>
   </si>
   <si>
     <t>done</t>
@@ -175,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +191,31 @@
       <family val="1"/>
       <charset val="163"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,12 +267,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -337,9 +348,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -356,9 +364,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -387,9 +392,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -401,6 +403,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,19 +717,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="32" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="12" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="14.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="23" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -721,17 +740,17 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -742,20 +761,20 @@
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="28">
+      <c r="F4" s="7"/>
+      <c r="G4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="25">
         <v>2010</v>
       </c>
     </row>
@@ -767,20 +786,20 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="29"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="66">
       <c r="A6" s="4">
@@ -790,20 +809,20 @@
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>0</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="29"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" ht="33">
       <c r="A7" s="4">
@@ -813,20 +832,20 @@
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="29"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="4">
@@ -836,20 +855,20 @@
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="29"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4">
@@ -859,20 +878,20 @@
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="29"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4">
@@ -882,20 +901,20 @@
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="29"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4">
@@ -905,20 +924,20 @@
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="29"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="4">
@@ -928,20 +947,20 @@
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>1</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="29"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4">
@@ -949,22 +968,22 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="29"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4">
@@ -972,22 +991,22 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="7">
+        <v>27</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="29"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4">
@@ -995,34 +1014,34 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>1</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="22"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="66">
       <c r="A17" s="4">
@@ -1030,22 +1049,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>1</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="28">
+      <c r="F17" s="7"/>
+      <c r="G17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="25">
         <v>2011</v>
       </c>
     </row>
@@ -1055,22 +1074,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>0.1</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="29"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:8" ht="33">
       <c r="A19" s="4">
@@ -1078,22 +1097,22 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="7">
+        <v>35</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="29"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="4">
@@ -1101,12 +1120,12 @@
         <v>17</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:8" ht="33">
       <c r="A21" s="4">
@@ -1114,22 +1133,24 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="7">
+        <v>43</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="6">
         <v>0</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="29"/>
+      <c r="F21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="33">
       <c r="A22" s="4">
@@ -1137,24 +1158,24 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="7">
+      <c r="D22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="6">
         <v>0</v>
       </c>
-      <c r="F22" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="23" t="s">
+      <c r="F22" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="29"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4">
@@ -1162,24 +1183,24 @@
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="6">
         <v>0.05</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="23" t="s">
+      <c r="F23" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="29"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" spans="1:8" ht="49.5">
       <c r="A24" s="4">
@@ -1187,24 +1208,24 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="7">
+      <c r="D24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="6">
         <v>0.05</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="23" t="s">
+      <c r="F24" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="29"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:8" ht="33">
       <c r="A25" s="4">
@@ -1212,22 +1233,24 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="7">
+        <v>41</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="6">
         <v>0.05</v>
       </c>
-      <c r="F25" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="29"/>
+      <c r="F25" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="4">
@@ -1235,22 +1258,24 @@
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="29"/>
+      <c r="G26" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:8" ht="49.5">
       <c r="A27" s="4">
@@ -1258,24 +1283,24 @@
         <v>24</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="6">
         <v>0</v>
       </c>
-      <c r="F27" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="23" t="s">
+      <c r="F27" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="33">
       <c r="A28" s="4">
@@ -1283,24 +1308,24 @@
         <v>25</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="7">
+      <c r="D28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="6">
         <v>0</v>
       </c>
-      <c r="F28" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" s="23" t="s">
+      <c r="F28" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="30"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
       <c r="A29" s="4">
@@ -1308,11 +1333,11 @@
         <v>26</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="24"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="4">
@@ -1320,11 +1345,11 @@
         <v>27</v>
       </c>
       <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="24"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="4">
@@ -1332,11 +1357,11 @@
         <v>28</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="24"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="4">
@@ -1344,11 +1369,11 @@
         <v>29</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="24"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="4">
@@ -1356,11 +1381,11 @@
         <v>30</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="24"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4">
@@ -1368,11 +1393,11 @@
         <v>31</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="24"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="4">
@@ -1380,11 +1405,11 @@
         <v>32</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="24"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="22"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="4">
@@ -1392,11 +1417,11 @@
         <v>33</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="24"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="4">
@@ -1404,11 +1429,11 @@
         <v>34</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="24"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="22"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="4">
@@ -1416,11 +1441,11 @@
         <v>35</v>
       </c>
       <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="24"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="22"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4">
@@ -1428,11 +1453,11 @@
         <v>36</v>
       </c>
       <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="24"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="4">
@@ -1440,11 +1465,11 @@
         <v>37</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="24"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4">
@@ -1452,128 +1477,128 @@
         <v>38</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="24"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="12"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="24"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="12"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="24"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="12"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="24"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="12"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="11"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="24"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="12"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="11"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="24"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="12"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="11"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="24"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="22"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="12"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="11"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="24"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="22"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="12"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="24"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="12"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="24"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="12"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="24"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="12"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="11"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="24"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="22"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="12"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="24"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="22"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="12"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="11"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="24"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
-update task file -update interact with user in QApage
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -424,15 +424,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -524,6 +515,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -838,610 +838,610 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="66">
-      <c r="A4" s="31">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="32">
         <v>0</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="36" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="48">
         <v>2010</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="66">
-      <c r="A5" s="31">
+      <c r="A5" s="28">
         <f xml:space="preserve"> A4 +1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="32">
         <v>0</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="36" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8" ht="66">
-      <c r="A6" s="31">
+      <c r="A6" s="28">
         <f xml:space="preserve"> A5 +1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="32">
         <v>0</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="36" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" ht="33">
-      <c r="A7" s="31">
+      <c r="A7" s="28">
         <f xml:space="preserve"> A6 +1</f>
         <v>4</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="32">
         <v>1</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="38" t="s">
+      <c r="F7" s="26"/>
+      <c r="G7" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="31">
+      <c r="A8" s="28">
         <f t="shared" ref="A8:A41" si="0" xml:space="preserve"> A7 +1</f>
         <v>5</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="32">
         <v>1</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="38" t="s">
+      <c r="F8" s="26"/>
+      <c r="G8" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="31">
+      <c r="A9" s="28">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="32">
         <v>1</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="38" t="s">
+      <c r="F9" s="26"/>
+      <c r="G9" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="31">
+      <c r="A10" s="28">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="38" t="s">
+      <c r="F10" s="26"/>
+      <c r="G10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="31">
+      <c r="A11" s="28">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="32">
         <v>1</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="38" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:8" ht="33">
-      <c r="A12" s="31">
+      <c r="A12" s="28">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="32">
         <v>1</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="38" t="s">
+      <c r="F12" s="26"/>
+      <c r="G12" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="49"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="31">
+      <c r="A13" s="28">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="32">
         <v>1</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="38" t="s">
+      <c r="F13" s="26"/>
+      <c r="G13" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="31">
+      <c r="A14" s="28">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="26"/>
+      <c r="G14" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="49"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="31">
+      <c r="A15" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="32">
         <v>1</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="38" t="s">
+      <c r="F15" s="26"/>
+      <c r="G15" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="18"/>
+      <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="31">
+      <c r="A16" s="28">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="45"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
     </row>
     <row r="17" spans="1:8" ht="66">
-      <c r="A17" s="31">
+      <c r="A17" s="28">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="32">
         <v>1</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="38" t="s">
+      <c r="F17" s="26"/>
+      <c r="G17" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="48">
         <v>2011</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="33">
-      <c r="A18" s="31">
+      <c r="A18" s="28">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="32">
         <v>0.1</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="36" t="s">
+      <c r="F18" s="26"/>
+      <c r="G18" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8" ht="33">
-      <c r="A19" s="31">
+      <c r="A19" s="28">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="38" t="s">
+      <c r="F19" s="26"/>
+      <c r="G19" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="49"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="31">
+      <c r="A20" s="28">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="17"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8" ht="33">
-      <c r="A21" s="31">
+      <c r="A21" s="28">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="32">
         <v>0.5</v>
       </c>
-      <c r="F21" s="47" t="s">
+      <c r="F21" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8" ht="33">
-      <c r="A22" s="31">
+      <c r="A22" s="28">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="32">
         <v>0</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="31">
+      <c r="A23" s="28">
         <f xml:space="preserve"> A22 +1</f>
         <v>20</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="32">
         <v>0.25</v>
       </c>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="G23" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="17"/>
+      <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8" ht="49.5">
-      <c r="A24" s="31">
+      <c r="A24" s="28">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="F24" s="49" t="s">
+      <c r="E24" s="32">
+        <v>1</v>
+      </c>
+      <c r="F24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="G24" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8" ht="33">
-      <c r="A25" s="31">
+      <c r="A25" s="28">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="32">
         <v>1</v>
       </c>
-      <c r="F25" s="50" t="s">
+      <c r="F25" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="31">
+      <c r="A26" s="28">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="32">
         <v>0.3</v>
       </c>
-      <c r="F26" s="47" t="s">
+      <c r="F26" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="17"/>
+      <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8" ht="49.5">
-      <c r="A27" s="31">
+      <c r="A27" s="28">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="32">
         <v>0</v>
       </c>
-      <c r="F27" s="50" t="s">
+      <c r="F27" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="17"/>
+      <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8" ht="33">
-      <c r="A28" s="31">
+      <c r="A28" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="35">
-        <v>0</v>
-      </c>
-      <c r="F28" s="50" t="s">
+      <c r="E28" s="32">
+        <v>1</v>
+      </c>
+      <c r="F28" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="G28" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="18"/>
+      <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A29" s="19">
+      <c r="A29" s="16">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="24"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3">

</xml_diff>

<commit_message>
-Update paper QABPSS.doc -update task
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -822,7 +822,7 @@
   <dimension ref="A3:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1296,7 +1296,7 @@
         <v>36</v>
       </c>
       <c r="E23" s="32">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="F23" s="46" t="s">
         <v>45</v>
@@ -1326,8 +1326,8 @@
       <c r="F24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>24</v>
+      <c r="G24" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="H24" s="49"/>
     </row>
@@ -1371,7 +1371,7 @@
         <v>36</v>
       </c>
       <c r="E26" s="32">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F26" s="44" t="s">
         <v>44</v>
@@ -1426,8 +1426,8 @@
       <c r="F28" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="45" t="s">
-        <v>24</v>
+      <c r="G28" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="H28" s="50"/>
     </row>

</xml_diff>

<commit_message>
-Update paper QABPSS.doc (100%)
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -822,7 +822,7 @@
   <dimension ref="A3:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1246,7 +1246,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="32">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F21" s="44" t="s">
         <v>44</v>
@@ -1296,13 +1296,13 @@
         <v>36</v>
       </c>
       <c r="E23" s="32">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F23" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="45" t="s">
-        <v>24</v>
+      <c r="G23" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="H23" s="49"/>
     </row>

</xml_diff>

<commit_message>
- Update All tasks in Tet holiday + Total : 10 tasks + Finish: 9 tasks + Cancel: 1 task + Delay : 0 task => Weldone work !
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Task No.</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>17/11</t>
-  </si>
-  <si>
-    <t>on processing</t>
   </si>
   <si>
     <t>Hoang &amp; Hung</t>
@@ -236,7 +233,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,12 +278,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -393,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -473,7 +464,7 @@
     <xf numFmtId="9" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,9 +496,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -821,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -876,9 +864,9 @@
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="48">
+        <v>31</v>
+      </c>
+      <c r="H4" s="47">
         <v>2010</v>
       </c>
     </row>
@@ -901,9 +889,9 @@
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="49"/>
+        <v>31</v>
+      </c>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:8" ht="66">
       <c r="A6" s="28">
@@ -924,9 +912,9 @@
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="49"/>
+        <v>31</v>
+      </c>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:8" ht="33">
       <c r="A7" s="28">
@@ -947,9 +935,9 @@
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="28">
@@ -970,9 +958,9 @@
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="28">
@@ -993,9 +981,9 @@
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="28">
@@ -1016,9 +1004,9 @@
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="28">
@@ -1039,9 +1027,9 @@
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H11" s="48"/>
     </row>
     <row r="12" spans="1:8" ht="33">
       <c r="A12" s="28">
@@ -1062,9 +1050,9 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="28">
@@ -1072,7 +1060,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>5</v>
@@ -1085,9 +1073,9 @@
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="28">
@@ -1095,22 +1083,22 @@
         <v>11</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="32">
         <v>1</v>
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="28">
@@ -1118,22 +1106,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="31" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>29</v>
       </c>
       <c r="E15" s="32">
         <v>1</v>
       </c>
       <c r="F15" s="26"/>
       <c r="G15" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="50"/>
+        <v>36</v>
+      </c>
+      <c r="H15" s="49"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="28">
@@ -1153,22 +1141,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="32">
         <v>1</v>
       </c>
       <c r="F17" s="26"/>
       <c r="G17" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="48">
+        <v>36</v>
+      </c>
+      <c r="H17" s="47">
         <v>2011</v>
       </c>
     </row>
@@ -1178,22 +1166,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="32">
         <v>0.1</v>
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="49"/>
+        <v>31</v>
+      </c>
+      <c r="H18" s="48"/>
     </row>
     <row r="19" spans="1:8" ht="33">
       <c r="A19" s="28">
@@ -1201,22 +1189,22 @@
         <v>16</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="32">
         <v>1</v>
       </c>
       <c r="F19" s="26"/>
       <c r="G19" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="28">
@@ -1229,7 +1217,7 @@
       <c r="E20" s="32"/>
       <c r="F20" s="26"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="49"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="1:8" ht="33">
       <c r="A21" s="28">
@@ -1237,24 +1225,24 @@
         <v>18</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="32">
         <v>1</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:8" ht="33">
       <c r="A22" s="28">
@@ -1262,24 +1250,24 @@
         <v>19</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="49"/>
+        <v>43</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="28">
@@ -1287,24 +1275,24 @@
         <v>20</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="32">
         <v>1</v>
       </c>
-      <c r="F23" s="46" t="s">
-        <v>45</v>
+      <c r="F23" s="45" t="s">
+        <v>44</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" ht="49.5">
       <c r="A24" s="28">
@@ -1312,24 +1300,24 @@
         <v>21</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="32">
         <v>1</v>
       </c>
-      <c r="F24" s="46" t="s">
-        <v>45</v>
+      <c r="F24" s="45" t="s">
+        <v>44</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="1:8" ht="33">
       <c r="A25" s="28">
@@ -1337,24 +1325,24 @@
         <v>22</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="32">
         <v>1</v>
       </c>
-      <c r="F25" s="47" t="s">
-        <v>46</v>
+      <c r="F25" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="49"/>
+        <v>36</v>
+      </c>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="28">
@@ -1362,24 +1350,24 @@
         <v>23</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F26" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="49"/>
+        <v>43</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="1:8" ht="49.5">
       <c r="A27" s="28">
@@ -1387,24 +1375,24 @@
         <v>24</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="32">
         <v>0</v>
       </c>
-      <c r="F27" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="49"/>
+      <c r="F27" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:8" ht="33">
       <c r="A28" s="28">
@@ -1412,24 +1400,24 @@
         <v>25</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="32">
         <v>1</v>
       </c>
-      <c r="F28" s="47" t="s">
-        <v>46</v>
+      <c r="F28" s="46" t="s">
+        <v>45</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="50"/>
+        <v>36</v>
+      </c>
+      <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
       <c r="A29" s="16">

</xml_diff>